<commit_message>
Exclude from analysis performance series where there is insufficient variation, and update results accordingly.
</commit_message>
<xml_diff>
--- a/data/outputs/full_results/summary_results_all.xlsx
+++ b/data/outputs/full_results/summary_results_all.xlsx
@@ -1249,10 +1249,10 @@
         </is>
       </c>
       <c r="B6">
-        <v>326</v>
+        <v>254</v>
       </c>
       <c r="C6">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D6">
         <v>95</v>
@@ -1267,19 +1267,19 @@
         <v>428</v>
       </c>
       <c r="H6">
-        <v>135.6319018404908</v>
+        <v>152.3503937007874</v>
       </c>
       <c r="I6">
-        <v>118.5867008787029</v>
+        <v>129.265450066412</v>
       </c>
       <c r="J6">
         <v>0</v>
       </c>
       <c r="K6">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="M6">
         <v>2</v>
@@ -1288,58 +1288,58 @@
         <v>13</v>
       </c>
       <c r="O6">
-        <v>2.177914110429448</v>
+        <v>2.704724409448819</v>
       </c>
       <c r="P6">
-        <v>3.105172350769744</v>
+        <v>3.323680950706546</v>
       </c>
       <c r="Q6">
         <v>0</v>
       </c>
       <c r="R6">
-        <v>3</v>
+        <v>8.25</v>
       </c>
       <c r="S6">
-        <v>13.5</v>
+        <v>17.5</v>
       </c>
       <c r="T6">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="U6">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="V6">
-        <v>16.15337423312883</v>
+        <v>18.65748031496063</v>
       </c>
       <c r="W6">
-        <v>13.78341604284975</v>
+        <v>12.70821849597764</v>
       </c>
       <c r="X6">
         <v>0</v>
       </c>
       <c r="Y6">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="Z6">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="AA6">
-        <v>35.75</v>
+        <v>39.75</v>
       </c>
       <c r="AB6">
         <v>79</v>
       </c>
       <c r="AC6">
-        <v>22.42024539877301</v>
+        <v>26.78740157480315</v>
       </c>
       <c r="AD6">
-        <v>17.82111335383857</v>
+        <v>16.95617691326643</v>
       </c>
       <c r="AE6">
         <v>0</v>
       </c>
       <c r="AF6">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="AG6">
         <v>2</v>
@@ -1351,16 +1351,16 @@
         <v>5</v>
       </c>
       <c r="AJ6">
-        <v>1.48159509202454</v>
+        <v>1.740157480314961</v>
       </c>
       <c r="AK6">
-        <v>1.14406773676837</v>
+        <v>1.083199757308116</v>
       </c>
       <c r="AL6">
         <v>0</v>
       </c>
       <c r="AM6">
-        <v>0.05263157894736842</v>
+        <v>0.4210526315789473</v>
       </c>
       <c r="AN6">
         <v>0.5</v>
@@ -1372,10 +1372,10 @@
         <v>1</v>
       </c>
       <c r="AQ6">
-        <v>0.4821947506803819</v>
+        <v>0.5617932626842698</v>
       </c>
       <c r="AR6">
-        <v>0.3477240501154034</v>
+        <v>0.3059352291189009</v>
       </c>
       <c r="AS6">
         <v>24.25</v>
@@ -1387,16 +1387,16 @@
         <v>47.5</v>
       </c>
       <c r="AV6">
-        <v>52</v>
+        <v>47.55555555555556</v>
       </c>
       <c r="AW6">
         <v>97</v>
       </c>
       <c r="AX6">
-        <v>49.57429327659389</v>
+        <v>45.34535278806932</v>
       </c>
       <c r="AY6">
-        <v>19.8272176415294</v>
+        <v>16.6245696389668</v>
       </c>
     </row>
     <row r="7">
@@ -1454,49 +1454,49 @@
         <v>0</v>
       </c>
       <c r="R7">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="S7">
-        <v>39.5</v>
+        <v>38</v>
       </c>
       <c r="T7">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="U7">
         <v>329</v>
       </c>
       <c r="V7">
-        <v>50.58282208588957</v>
+        <v>48.3282208588957</v>
       </c>
       <c r="W7">
-        <v>60.76874864355555</v>
+        <v>61.82814595232369</v>
       </c>
       <c r="X7">
         <v>0</v>
       </c>
       <c r="Y7">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="Z7">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AA7">
-        <v>82</v>
+        <v>81.75</v>
       </c>
       <c r="AB7">
         <v>395</v>
       </c>
       <c r="AC7">
-        <v>87.07668711656441</v>
+        <v>82.88343558282209</v>
       </c>
       <c r="AD7">
-        <v>97.19124814702015</v>
+        <v>99.74264685528911</v>
       </c>
       <c r="AE7">
         <v>0</v>
       </c>
       <c r="AF7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG7">
         <v>3</v>
@@ -1508,10 +1508,10 @@
         <v>16</v>
       </c>
       <c r="AJ7">
-        <v>3.524539877300613</v>
+        <v>3.285276073619632</v>
       </c>
       <c r="AK7">
-        <v>2.756421136173384</v>
+        <v>2.932297248629149</v>
       </c>
       <c r="AL7">
         <v>0</v>
@@ -1563,10 +1563,10 @@
         </is>
       </c>
       <c r="B8">
-        <v>326</v>
+        <v>254</v>
       </c>
       <c r="C8">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D8">
         <v>95</v>
@@ -1581,10 +1581,10 @@
         <v>428</v>
       </c>
       <c r="H8">
-        <v>135.6319018404908</v>
+        <v>152.3503937007874</v>
       </c>
       <c r="I8">
-        <v>118.5867008787029</v>
+        <v>129.265450066412</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1611,43 +1611,43 @@
         <v>0</v>
       </c>
       <c r="R8">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="S8">
-        <v>37.5</v>
+        <v>46</v>
       </c>
       <c r="T8">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="U8">
         <v>316</v>
       </c>
       <c r="V8">
-        <v>49.63496932515337</v>
+        <v>61.65354330708661</v>
       </c>
       <c r="W8">
-        <v>58.19441055236764</v>
+        <v>60.31968562220263</v>
       </c>
       <c r="X8">
         <v>0</v>
       </c>
       <c r="Y8">
-        <v>30.25</v>
+        <v>47</v>
       </c>
       <c r="Z8">
-        <v>52.5</v>
+        <v>61</v>
       </c>
       <c r="AA8">
-        <v>70.75</v>
+        <v>76</v>
       </c>
       <c r="AB8">
         <v>366</v>
       </c>
       <c r="AC8">
-        <v>73.63803680981596</v>
+        <v>90.72834645669292</v>
       </c>
       <c r="AD8">
-        <v>82.64994370780452</v>
+        <v>85.74113664665592</v>
       </c>
       <c r="AE8">
         <v>0</v>
@@ -1656,19 +1656,19 @@
         <v>2</v>
       </c>
       <c r="AG8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AI8">
         <v>13</v>
       </c>
       <c r="AJ8">
-        <v>2.861963190184049</v>
+        <v>3.44488188976378</v>
       </c>
       <c r="AK8">
-        <v>2.492319490297701</v>
+        <v>2.47415761722017</v>
       </c>
       <c r="AL8">
         <v>0</v>
@@ -1692,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="AS8">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AT8">
         <v>95</v>
@@ -1707,10 +1707,10 @@
         <v>428</v>
       </c>
       <c r="AX8">
-        <v>135.6319018404908</v>
+        <v>152.3503937007874</v>
       </c>
       <c r="AY8">
-        <v>118.5867008787029</v>
+        <v>129.265450066412</v>
       </c>
     </row>
     <row r="9">
@@ -1720,10 +1720,10 @@
         </is>
       </c>
       <c r="B9">
-        <v>326</v>
+        <v>254</v>
       </c>
       <c r="C9">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D9">
         <v>95</v>
@@ -1738,10 +1738,10 @@
         <v>428</v>
       </c>
       <c r="H9">
-        <v>135.6319018404908</v>
+        <v>152.3503937007874</v>
       </c>
       <c r="I9">
-        <v>118.5867008787029</v>
+        <v>129.265450066412</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1759,61 +1759,61 @@
         <v>16</v>
       </c>
       <c r="O9">
-        <v>2.650306748466257</v>
+        <v>3.291338582677165</v>
       </c>
       <c r="P9">
-        <v>3.619662104640391</v>
+        <v>3.854283046930683</v>
       </c>
       <c r="Q9">
         <v>0</v>
       </c>
       <c r="R9">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="S9">
-        <v>12.5</v>
+        <v>17</v>
       </c>
       <c r="T9">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="U9">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="V9">
-        <v>14.87116564417178</v>
+        <v>17.26771653543307</v>
       </c>
       <c r="W9">
-        <v>12.79165460603787</v>
+        <v>11.70821057058593</v>
       </c>
       <c r="X9">
         <v>0</v>
       </c>
       <c r="Y9">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="Z9">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="AA9">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="AB9">
         <v>60</v>
       </c>
       <c r="AC9">
-        <v>20.65030674846626</v>
+        <v>24.72834645669291</v>
       </c>
       <c r="AD9">
-        <v>16.4498431107155</v>
+        <v>15.69374084158438</v>
       </c>
       <c r="AE9">
         <v>0</v>
       </c>
       <c r="AF9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH9">
         <v>2</v>
@@ -1822,19 +1822,19 @@
         <v>4</v>
       </c>
       <c r="AJ9">
-        <v>1.368098159509203</v>
+        <v>1.598425196850394</v>
       </c>
       <c r="AK9">
-        <v>1.034524373596791</v>
+        <v>0.9679434416535295</v>
       </c>
       <c r="AL9">
         <v>0</v>
       </c>
       <c r="AM9">
-        <v>0.4342105263157894</v>
+        <v>0.5</v>
       </c>
       <c r="AN9">
-        <v>0.6666666666666666</v>
+        <v>0.6842105263157895</v>
       </c>
       <c r="AO9">
         <v>1</v>
@@ -1843,10 +1843,10 @@
         <v>1</v>
       </c>
       <c r="AQ9">
-        <v>0.6204506665436598</v>
+        <v>0.7274288082410751</v>
       </c>
       <c r="AR9">
-        <v>0.371205094110962</v>
+        <v>0.288957936411547</v>
       </c>
       <c r="AS9">
         <v>24.25</v>
@@ -1855,19 +1855,19 @@
         <v>31.66666666666667</v>
       </c>
       <c r="AU9">
-        <v>32.33333333333334</v>
+        <v>31.83333333333334</v>
       </c>
       <c r="AV9">
-        <v>47.54166666666667</v>
+        <v>47.5</v>
       </c>
       <c r="AW9">
         <v>95</v>
       </c>
       <c r="AX9">
-        <v>43.49775370285114</v>
+        <v>38.01680199657272</v>
       </c>
       <c r="AY9">
-        <v>18.79290625264466</v>
+        <v>12.58556745886677</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data in line with fixes of issues #6 through #8.
</commit_message>
<xml_diff>
--- a/data/outputs/full_results/summary_results_all.xlsx
+++ b/data/outputs/full_results/summary_results_all.xlsx
@@ -621,7 +621,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="C2">
         <v>48</v>
@@ -639,10 +639,10 @@
         <v>428</v>
       </c>
       <c r="H2">
-        <v>135.6319018404908</v>
+        <v>137.0601265822785</v>
       </c>
       <c r="I2">
-        <v>118.5867008787029</v>
+        <v>120.1679757883243</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -660,10 +660,10 @@
         <v>13</v>
       </c>
       <c r="O2">
-        <v>2.460122699386503</v>
+        <v>2.531645569620253</v>
       </c>
       <c r="P2">
-        <v>3.285858555451984</v>
+        <v>3.311683763132613</v>
       </c>
       <c r="Q2">
         <v>0</v>
@@ -681,31 +681,31 @@
         <v>110</v>
       </c>
       <c r="V2">
-        <v>19.47239263803681</v>
+        <v>19.52215189873418</v>
       </c>
       <c r="W2">
-        <v>13.75178327275214</v>
+        <v>12.41847637009594</v>
       </c>
       <c r="X2">
         <v>0</v>
       </c>
       <c r="Y2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Z2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AA2">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AB2">
         <v>127</v>
       </c>
       <c r="AC2">
-        <v>28.72085889570552</v>
+        <v>29.5</v>
       </c>
       <c r="AD2">
-        <v>17.58772282977394</v>
+        <v>17.23608249233391</v>
       </c>
       <c r="AE2">
         <v>0</v>
@@ -723,16 +723,16 @@
         <v>8</v>
       </c>
       <c r="AJ2">
-        <v>1.831288343558282</v>
+        <v>1.882911392405063</v>
       </c>
       <c r="AK2">
-        <v>1.173713185900208</v>
+        <v>1.152867675771185</v>
       </c>
       <c r="AL2">
         <v>0</v>
       </c>
       <c r="AM2">
-        <v>0.4736842105263158</v>
+        <v>0.5</v>
       </c>
       <c r="AN2">
         <v>0.5</v>
@@ -744,10 +744,10 @@
         <v>1</v>
       </c>
       <c r="AQ2">
-        <v>0.5869620369943263</v>
+        <v>0.6023722280384506</v>
       </c>
       <c r="AR2">
-        <v>0.3450647908899001</v>
+        <v>0.3373627583929834</v>
       </c>
       <c r="AS2">
         <v>24</v>
@@ -756,7 +756,7 @@
         <v>31.66666666666667</v>
       </c>
       <c r="AU2">
-        <v>41.5</v>
+        <v>38.90909090909091</v>
       </c>
       <c r="AV2">
         <v>47.5</v>
@@ -765,10 +765,10 @@
         <v>97</v>
       </c>
       <c r="AX2">
-        <v>44.19926966353346</v>
+        <v>43.01886680478453</v>
       </c>
       <c r="AY2">
-        <v>16.54974338533422</v>
+        <v>14.97922458263611</v>
       </c>
     </row>
     <row r="3">
@@ -778,7 +778,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="C3">
         <v>48</v>
@@ -796,10 +796,10 @@
         <v>428</v>
       </c>
       <c r="H3">
-        <v>135.6319018404908</v>
+        <v>137.0601265822785</v>
       </c>
       <c r="I3">
-        <v>118.5867008787029</v>
+        <v>120.1679757883243</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -826,31 +826,31 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="S3">
-        <v>29</v>
+        <v>29.5</v>
       </c>
       <c r="T3">
-        <v>57</v>
+        <v>57.25</v>
       </c>
       <c r="U3">
         <v>237</v>
       </c>
       <c r="V3">
-        <v>42.83742331288344</v>
+        <v>43.62341772151899</v>
       </c>
       <c r="W3">
-        <v>38.43773720369417</v>
+        <v>38.24732324730301</v>
       </c>
       <c r="X3">
         <v>0</v>
       </c>
       <c r="Y3">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="Z3">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="AA3">
         <v>85</v>
@@ -859,10 +859,10 @@
         <v>378</v>
       </c>
       <c r="AC3">
-        <v>88.74539877300613</v>
+        <v>90.98417721518987</v>
       </c>
       <c r="AD3">
-        <v>83.5693699518441</v>
+        <v>83.66799317647113</v>
       </c>
       <c r="AE3">
         <v>0</v>
@@ -880,10 +880,10 @@
         <v>18</v>
       </c>
       <c r="AJ3">
-        <v>4.095092024539877</v>
+        <v>4.218354430379747</v>
       </c>
       <c r="AK3">
-        <v>3.993091012944643</v>
+        <v>3.993619333229222</v>
       </c>
       <c r="AL3">
         <v>0</v>
@@ -922,10 +922,10 @@
         <v>428</v>
       </c>
       <c r="AX3">
-        <v>135.6319018404908</v>
+        <v>137.0601265822785</v>
       </c>
       <c r="AY3">
-        <v>118.5867008787029</v>
+        <v>120.1679757883243</v>
       </c>
     </row>
     <row r="4">
@@ -935,7 +935,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="C4">
         <v>48</v>
@@ -953,10 +953,10 @@
         <v>428</v>
       </c>
       <c r="H4">
-        <v>135.6319018404908</v>
+        <v>137.0601265822785</v>
       </c>
       <c r="I4">
-        <v>118.5867008787029</v>
+        <v>120.1679757883243</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -983,31 +983,31 @@
         <v>0</v>
       </c>
       <c r="R4">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="S4">
-        <v>40.5</v>
+        <v>41</v>
       </c>
       <c r="T4">
-        <v>57</v>
+        <v>57.25</v>
       </c>
       <c r="U4">
         <v>408</v>
       </c>
       <c r="V4">
-        <v>54.15950920245399</v>
+        <v>55.30696202531646</v>
       </c>
       <c r="W4">
-        <v>55.30273899244114</v>
+        <v>55.42210964128501</v>
       </c>
       <c r="X4">
         <v>0</v>
       </c>
       <c r="Y4">
-        <v>41.25</v>
+        <v>43</v>
       </c>
       <c r="Z4">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AA4">
         <v>71</v>
@@ -1016,10 +1016,10 @@
         <v>423</v>
       </c>
       <c r="AC4">
-        <v>84.07055214723927</v>
+        <v>86.1613924050633</v>
       </c>
       <c r="AD4">
-        <v>87.79240158641055</v>
+        <v>88.13580374369498</v>
       </c>
       <c r="AE4">
         <v>0</v>
@@ -1037,10 +1037,10 @@
         <v>17</v>
       </c>
       <c r="AJ4">
-        <v>3.503067484662577</v>
+        <v>3.607594936708861</v>
       </c>
       <c r="AK4">
-        <v>3.429059944073185</v>
+        <v>3.430647017577352</v>
       </c>
       <c r="AL4">
         <v>0</v>
@@ -1079,10 +1079,10 @@
         <v>428</v>
       </c>
       <c r="AX4">
-        <v>135.6319018404908</v>
+        <v>137.0601265822785</v>
       </c>
       <c r="AY4">
-        <v>118.5867008787029</v>
+        <v>120.1679757883243</v>
       </c>
     </row>
     <row r="5">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="C5">
         <v>48</v>
@@ -1110,10 +1110,10 @@
         <v>428</v>
       </c>
       <c r="H5">
-        <v>135.6319018404908</v>
+        <v>137.0601265822785</v>
       </c>
       <c r="I5">
-        <v>118.5867008787029</v>
+        <v>120.1679757883243</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -1131,16 +1131,16 @@
         <v>18</v>
       </c>
       <c r="O5">
-        <v>3.420245398773006</v>
+        <v>3.522151898734177</v>
       </c>
       <c r="P5">
-        <v>4.560508197176848</v>
+        <v>4.594974804051639</v>
       </c>
       <c r="Q5">
         <v>0</v>
       </c>
       <c r="R5">
-        <v>9</v>
+        <v>9.75</v>
       </c>
       <c r="S5">
         <v>16</v>
@@ -1149,34 +1149,34 @@
         <v>25</v>
       </c>
       <c r="U5">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="V5">
-        <v>17.6717791411043</v>
+        <v>17.66455696202532</v>
       </c>
       <c r="W5">
-        <v>12.58398009291033</v>
+        <v>11.07097492702609</v>
       </c>
       <c r="X5">
         <v>0</v>
       </c>
       <c r="Y5">
-        <v>18.25</v>
+        <v>19</v>
       </c>
       <c r="Z5">
-        <v>29.5</v>
+        <v>30</v>
       </c>
       <c r="AA5">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AB5">
         <v>71</v>
       </c>
       <c r="AC5">
-        <v>29.37730061349693</v>
+        <v>30.17721518987342</v>
       </c>
       <c r="AD5">
-        <v>15.66265445864436</v>
+        <v>15.16471216599101</v>
       </c>
       <c r="AE5">
         <v>0</v>
@@ -1194,10 +1194,10 @@
         <v>4</v>
       </c>
       <c r="AJ5">
-        <v>1.576687116564417</v>
+        <v>1.620253164556962</v>
       </c>
       <c r="AK5">
-        <v>0.9308107666659206</v>
+        <v>0.9092651485168747</v>
       </c>
       <c r="AL5">
         <v>0</v>
@@ -1215,10 +1215,10 @@
         <v>1</v>
       </c>
       <c r="AQ5">
-        <v>0.8128911235143073</v>
+        <v>0.8354509691951397</v>
       </c>
       <c r="AR5">
-        <v>0.2773727457289895</v>
+        <v>0.2479190750366284</v>
       </c>
       <c r="AS5">
         <v>22.52631578947368</v>
@@ -1233,13 +1233,13 @@
         <v>32.33333333333334</v>
       </c>
       <c r="AW5">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="AX5">
-        <v>34.63994295315545</v>
+        <v>33.1570297554705</v>
       </c>
       <c r="AY5">
-        <v>11.31852132713244</v>
+        <v>6.900392719654174</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Amend 3b to periodMin = 8 rather than no minimum period. Update results.
</commit_message>
<xml_diff>
--- a/data/outputs/full_results/summary_results_all.xlsx
+++ b/data/outputs/full_results/summary_results_all.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AY9"/>
+  <dimension ref="A1:AY11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1245,14 +1245,14 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>P algorithm</t>
+          <t>C naive3b</t>
         </is>
       </c>
       <c r="B6">
-        <v>254</v>
+        <v>316</v>
       </c>
       <c r="C6">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6">
         <v>95</v>
@@ -1267,149 +1267,149 @@
         <v>428</v>
       </c>
       <c r="H6">
-        <v>152.3503937007874</v>
+        <v>137.0601265822785</v>
       </c>
       <c r="I6">
-        <v>129.265450066412</v>
+        <v>120.1679757883243</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>5</v>
+      </c>
+      <c r="M6">
+        <v>6</v>
+      </c>
+      <c r="N6">
+        <v>38</v>
+      </c>
+      <c r="O6">
+        <v>7.981012658227848</v>
+      </c>
+      <c r="P6">
+        <v>8.594181508245255</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
         <v>1</v>
       </c>
-      <c r="L6">
+      <c r="T6">
+        <v>3</v>
+      </c>
+      <c r="U6">
+        <v>45</v>
+      </c>
+      <c r="V6">
+        <v>2.512658227848101</v>
+      </c>
+      <c r="W6">
+        <v>4.48098251948876</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>17</v>
+      </c>
+      <c r="AC6">
+        <v>1.069620253164557</v>
+      </c>
+      <c r="AD6">
+        <v>3.073939798870591</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>2</v>
+      </c>
+      <c r="AJ6">
+        <v>0.120253164556962</v>
+      </c>
+      <c r="AK6">
+        <v>0.3447123472852491</v>
+      </c>
+      <c r="AL6">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="AM6">
         <v>1.5</v>
       </c>
-      <c r="M6">
-        <v>2</v>
-      </c>
-      <c r="N6">
-        <v>13</v>
-      </c>
-      <c r="O6">
-        <v>2.704724409448819</v>
-      </c>
-      <c r="P6">
-        <v>3.323680950706546</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>8.25</v>
-      </c>
-      <c r="S6">
-        <v>17.5</v>
-      </c>
-      <c r="T6">
-        <v>28</v>
-      </c>
-      <c r="U6">
-        <v>59</v>
-      </c>
-      <c r="V6">
-        <v>18.65748031496063</v>
-      </c>
-      <c r="W6">
-        <v>12.70821849597764</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6">
-        <v>14</v>
-      </c>
-      <c r="Z6">
-        <v>29</v>
-      </c>
-      <c r="AA6">
-        <v>39.75</v>
-      </c>
-      <c r="AB6">
-        <v>79</v>
-      </c>
-      <c r="AC6">
-        <v>26.78740157480315</v>
-      </c>
-      <c r="AD6">
-        <v>16.95617691326643</v>
-      </c>
-      <c r="AE6">
-        <v>0</v>
-      </c>
-      <c r="AF6">
-        <v>1</v>
-      </c>
-      <c r="AG6">
-        <v>2</v>
-      </c>
-      <c r="AH6">
-        <v>2</v>
-      </c>
-      <c r="AI6">
-        <v>5</v>
-      </c>
-      <c r="AJ6">
-        <v>1.740157480314961</v>
-      </c>
-      <c r="AK6">
-        <v>1.083199757308116</v>
-      </c>
-      <c r="AL6">
-        <v>0</v>
-      </c>
-      <c r="AM6">
-        <v>0.4210526315789473</v>
-      </c>
       <c r="AN6">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="AO6">
-        <v>0.6666666666666666</v>
+        <v>3</v>
       </c>
       <c r="AP6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AQ6">
-        <v>0.5617932626842698</v>
+        <v>2.290964753656293</v>
       </c>
       <c r="AR6">
-        <v>0.3059352291189009</v>
+        <v>0.9224471218358076</v>
       </c>
       <c r="AS6">
-        <v>24.25</v>
+        <v>9.333333333333334</v>
       </c>
       <c r="AT6">
-        <v>32.33333333333334</v>
+        <v>13.57142857142857</v>
       </c>
       <c r="AU6">
-        <v>47.5</v>
+        <v>15.83333333333333</v>
       </c>
       <c r="AV6">
-        <v>47.55555555555556</v>
+        <v>19</v>
       </c>
       <c r="AW6">
-        <v>97</v>
+        <v>34</v>
       </c>
       <c r="AX6">
-        <v>45.34535278806932</v>
+        <v>16.53393065646352</v>
       </c>
       <c r="AY6">
-        <v>16.6245696389668</v>
+        <v>4.521254120415229</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>P naive1</t>
+          <t>P algorithm</t>
         </is>
       </c>
       <c r="B7">
-        <v>326</v>
+        <v>254</v>
       </c>
       <c r="C7">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D7">
         <v>95</v>
@@ -1424,73 +1424,73 @@
         <v>428</v>
       </c>
       <c r="H7">
-        <v>135.6319018404908</v>
+        <v>152.3503937007874</v>
       </c>
       <c r="I7">
-        <v>118.5867008787029</v>
+        <v>129.265450066412</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>2.704724409448819</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>3.323680950706546</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7">
-        <v>7</v>
+        <v>8.25</v>
       </c>
       <c r="S7">
-        <v>38</v>
+        <v>17.5</v>
       </c>
       <c r="T7">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="U7">
-        <v>329</v>
+        <v>59</v>
       </c>
       <c r="V7">
-        <v>48.3282208588957</v>
+        <v>18.65748031496063</v>
       </c>
       <c r="W7">
-        <v>61.82814595232369</v>
+        <v>12.70821849597764</v>
       </c>
       <c r="X7">
         <v>0</v>
       </c>
       <c r="Y7">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="Z7">
-        <v>64</v>
+        <v>29</v>
       </c>
       <c r="AA7">
-        <v>81.75</v>
+        <v>39.75</v>
       </c>
       <c r="AB7">
-        <v>395</v>
+        <v>79</v>
       </c>
       <c r="AC7">
-        <v>82.88343558282209</v>
+        <v>26.78740157480315</v>
       </c>
       <c r="AD7">
-        <v>99.74264685528911</v>
+        <v>16.95617691326643</v>
       </c>
       <c r="AE7">
         <v>0</v>
@@ -1499,74 +1499,74 @@
         <v>1</v>
       </c>
       <c r="AG7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AH7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AI7">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="AJ7">
-        <v>3.285276073619632</v>
+        <v>1.740157480314961</v>
       </c>
       <c r="AK7">
-        <v>2.932297248629149</v>
+        <v>1.083199757308116</v>
       </c>
       <c r="AL7">
         <v>0</v>
       </c>
       <c r="AM7">
-        <v>0</v>
+        <v>0.4210526315789473</v>
       </c>
       <c r="AN7">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="AO7">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AP7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ7">
-        <v>0</v>
+        <v>0.5617932626842698</v>
       </c>
       <c r="AR7">
-        <v>0</v>
+        <v>0.3059352291189009</v>
       </c>
       <c r="AS7">
-        <v>48</v>
+        <v>24.25</v>
       </c>
       <c r="AT7">
-        <v>95</v>
+        <v>32.33333333333334</v>
       </c>
       <c r="AU7">
-        <v>95</v>
+        <v>47.5</v>
       </c>
       <c r="AV7">
+        <v>47.55555555555556</v>
+      </c>
+      <c r="AW7">
         <v>97</v>
       </c>
-      <c r="AW7">
-        <v>428</v>
-      </c>
       <c r="AX7">
-        <v>135.6319018404908</v>
+        <v>45.34535278806932</v>
       </c>
       <c r="AY7">
-        <v>118.5867008787029</v>
+        <v>16.6245696389668</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>P naive2</t>
+          <t>P naive1</t>
         </is>
       </c>
       <c r="B8">
-        <v>254</v>
+        <v>326</v>
       </c>
       <c r="C8">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8">
         <v>95</v>
@@ -1581,10 +1581,10 @@
         <v>428</v>
       </c>
       <c r="H8">
-        <v>152.3503937007874</v>
+        <v>135.6319018404908</v>
       </c>
       <c r="I8">
-        <v>129.265450066412</v>
+        <v>118.5867008787029</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1611,49 +1611,49 @@
         <v>0</v>
       </c>
       <c r="R8">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="S8">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="T8">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="U8">
-        <v>316</v>
+        <v>329</v>
       </c>
       <c r="V8">
-        <v>61.65354330708661</v>
+        <v>48.3282208588957</v>
       </c>
       <c r="W8">
-        <v>60.31968562220263</v>
+        <v>61.82814595232369</v>
       </c>
       <c r="X8">
         <v>0</v>
       </c>
       <c r="Y8">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="Z8">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="AA8">
-        <v>76</v>
+        <v>81.75</v>
       </c>
       <c r="AB8">
-        <v>366</v>
+        <v>395</v>
       </c>
       <c r="AC8">
-        <v>90.72834645669292</v>
+        <v>82.88343558282209</v>
       </c>
       <c r="AD8">
-        <v>85.74113664665592</v>
+        <v>99.74264685528911</v>
       </c>
       <c r="AE8">
         <v>0</v>
       </c>
       <c r="AF8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG8">
         <v>3</v>
@@ -1662,13 +1662,13 @@
         <v>4</v>
       </c>
       <c r="AI8">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="AJ8">
-        <v>3.44488188976378</v>
+        <v>3.285276073619632</v>
       </c>
       <c r="AK8">
-        <v>2.47415761722017</v>
+        <v>2.932297248629149</v>
       </c>
       <c r="AL8">
         <v>0</v>
@@ -1692,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="AS8">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AT8">
         <v>95</v>
@@ -1707,16 +1707,16 @@
         <v>428</v>
       </c>
       <c r="AX8">
-        <v>152.3503937007874</v>
+        <v>135.6319018404908</v>
       </c>
       <c r="AY8">
-        <v>129.265450066412</v>
+        <v>118.5867008787029</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>P naive3</t>
+          <t>P naive2</t>
         </is>
       </c>
       <c r="B9">
@@ -1747,127 +1747,441 @@
         <v>0</v>
       </c>
       <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>30</v>
+      </c>
+      <c r="S9">
+        <v>46</v>
+      </c>
+      <c r="T9">
+        <v>60</v>
+      </c>
+      <c r="U9">
+        <v>316</v>
+      </c>
+      <c r="V9">
+        <v>61.65354330708661</v>
+      </c>
+      <c r="W9">
+        <v>60.31968562220263</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>47</v>
+      </c>
+      <c r="Z9">
+        <v>61</v>
+      </c>
+      <c r="AA9">
+        <v>76</v>
+      </c>
+      <c r="AB9">
+        <v>366</v>
+      </c>
+      <c r="AC9">
+        <v>90.72834645669292</v>
+      </c>
+      <c r="AD9">
+        <v>85.74113664665592</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+      <c r="AF9">
+        <v>2</v>
+      </c>
+      <c r="AG9">
+        <v>3</v>
+      </c>
+      <c r="AH9">
+        <v>4</v>
+      </c>
+      <c r="AI9">
+        <v>13</v>
+      </c>
+      <c r="AJ9">
+        <v>3.44488188976378</v>
+      </c>
+      <c r="AK9">
+        <v>2.47415761722017</v>
+      </c>
+      <c r="AL9">
+        <v>0</v>
+      </c>
+      <c r="AM9">
+        <v>0</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9">
+        <v>0</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+      <c r="AQ9">
+        <v>0</v>
+      </c>
+      <c r="AR9">
+        <v>0</v>
+      </c>
+      <c r="AS9">
+        <v>49</v>
+      </c>
+      <c r="AT9">
+        <v>95</v>
+      </c>
+      <c r="AU9">
+        <v>95</v>
+      </c>
+      <c r="AV9">
+        <v>97</v>
+      </c>
+      <c r="AW9">
+        <v>428</v>
+      </c>
+      <c r="AX9">
+        <v>152.3503937007874</v>
+      </c>
+      <c r="AY9">
+        <v>129.265450066412</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>P naive3</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>254</v>
+      </c>
+      <c r="C10">
+        <v>49</v>
+      </c>
+      <c r="D10">
+        <v>95</v>
+      </c>
+      <c r="E10">
+        <v>95</v>
+      </c>
+      <c r="F10">
+        <v>97</v>
+      </c>
+      <c r="G10">
+        <v>428</v>
+      </c>
+      <c r="H10">
+        <v>152.3503937007874</v>
+      </c>
+      <c r="I10">
+        <v>129.265450066412</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
         <v>1</v>
       </c>
-      <c r="L9">
-        <v>2</v>
-      </c>
-      <c r="M9">
-        <v>2</v>
-      </c>
-      <c r="N9">
+      <c r="L10">
+        <v>2</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="N10">
         <v>16</v>
       </c>
-      <c r="O9">
+      <c r="O10">
         <v>3.291338582677165</v>
       </c>
-      <c r="P9">
+      <c r="P10">
         <v>3.854283046930683</v>
       </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
         <v>7</v>
       </c>
-      <c r="S9">
+      <c r="S10">
         <v>17</v>
       </c>
-      <c r="T9">
+      <c r="T10">
         <v>26</v>
       </c>
-      <c r="U9">
+      <c r="U10">
         <v>51</v>
       </c>
-      <c r="V9">
+      <c r="V10">
         <v>17.26771653543307</v>
       </c>
-      <c r="W9">
+      <c r="W10">
         <v>11.70821057058593</v>
       </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
-      <c r="Y9">
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
         <v>11</v>
       </c>
-      <c r="Z9">
+      <c r="Z10">
         <v>26</v>
       </c>
-      <c r="AA9">
+      <c r="AA10">
         <v>37</v>
       </c>
-      <c r="AB9">
+      <c r="AB10">
         <v>60</v>
       </c>
-      <c r="AC9">
+      <c r="AC10">
         <v>24.72834645669291</v>
       </c>
-      <c r="AD9">
+      <c r="AD10">
         <v>15.69374084158438</v>
       </c>
-      <c r="AE9">
-        <v>0</v>
-      </c>
-      <c r="AF9">
+      <c r="AE10">
+        <v>0</v>
+      </c>
+      <c r="AF10">
         <v>1</v>
       </c>
-      <c r="AG9">
-        <v>2</v>
-      </c>
-      <c r="AH9">
-        <v>2</v>
-      </c>
-      <c r="AI9">
+      <c r="AG10">
+        <v>2</v>
+      </c>
+      <c r="AH10">
+        <v>2</v>
+      </c>
+      <c r="AI10">
         <v>4</v>
       </c>
-      <c r="AJ9">
+      <c r="AJ10">
         <v>1.598425196850394</v>
       </c>
-      <c r="AK9">
+      <c r="AK10">
         <v>0.9679434416535295</v>
       </c>
-      <c r="AL9">
-        <v>0</v>
-      </c>
-      <c r="AM9">
+      <c r="AL10">
+        <v>0</v>
+      </c>
+      <c r="AM10">
         <v>0.5</v>
       </c>
-      <c r="AN9">
+      <c r="AN10">
         <v>0.6842105263157895</v>
       </c>
-      <c r="AO9">
+      <c r="AO10">
         <v>1</v>
       </c>
-      <c r="AP9">
+      <c r="AP10">
         <v>1</v>
       </c>
-      <c r="AQ9">
+      <c r="AQ10">
         <v>0.7274288082410751</v>
       </c>
-      <c r="AR9">
+      <c r="AR10">
         <v>0.288957936411547</v>
       </c>
-      <c r="AS9">
+      <c r="AS10">
         <v>24.25</v>
       </c>
-      <c r="AT9">
+      <c r="AT10">
         <v>31.66666666666667</v>
       </c>
-      <c r="AU9">
+      <c r="AU10">
         <v>31.83333333333334</v>
       </c>
-      <c r="AV9">
+      <c r="AV10">
         <v>47.5</v>
       </c>
-      <c r="AW9">
-        <v>95</v>
-      </c>
-      <c r="AX9">
+      <c r="AW10">
+        <v>95</v>
+      </c>
+      <c r="AX10">
         <v>38.01680199657272</v>
       </c>
-      <c r="AY9">
+      <c r="AY10">
         <v>12.58556745886677</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>P naive3b</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>254</v>
+      </c>
+      <c r="C11">
+        <v>49</v>
+      </c>
+      <c r="D11">
+        <v>95</v>
+      </c>
+      <c r="E11">
+        <v>95</v>
+      </c>
+      <c r="F11">
+        <v>97</v>
+      </c>
+      <c r="G11">
+        <v>428</v>
+      </c>
+      <c r="H11">
+        <v>152.3503937007874</v>
+      </c>
+      <c r="I11">
+        <v>129.265450066412</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>4</v>
+      </c>
+      <c r="L11">
+        <v>6</v>
+      </c>
+      <c r="M11">
+        <v>7</v>
+      </c>
+      <c r="N11">
+        <v>35</v>
+      </c>
+      <c r="O11">
+        <v>7.377952755905512</v>
+      </c>
+      <c r="P11">
+        <v>5.779107982453519</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>2</v>
+      </c>
+      <c r="T11">
+        <v>5</v>
+      </c>
+      <c r="U11">
+        <v>17</v>
+      </c>
+      <c r="V11">
+        <v>3.216535433070866</v>
+      </c>
+      <c r="W11">
+        <v>3.275909523513953</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>19</v>
+      </c>
+      <c r="AC11">
+        <v>1.803149606299213</v>
+      </c>
+      <c r="AD11">
+        <v>3.905078015807789</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <v>2</v>
+      </c>
+      <c r="AJ11">
+        <v>0.2007874015748032</v>
+      </c>
+      <c r="AK11">
+        <v>0.4299087251214076</v>
+      </c>
+      <c r="AL11">
+        <v>0</v>
+      </c>
+      <c r="AM11">
+        <v>1.333333333333333</v>
+      </c>
+      <c r="AN11">
+        <v>2</v>
+      </c>
+      <c r="AO11">
+        <v>3</v>
+      </c>
+      <c r="AP11">
+        <v>4.5</v>
+      </c>
+      <c r="AQ11">
+        <v>2.192074674876167</v>
+      </c>
+      <c r="AR11">
+        <v>1.038702278113778</v>
+      </c>
+      <c r="AS11">
+        <v>9.5</v>
+      </c>
+      <c r="AT11">
+        <v>13.57142857142857</v>
+      </c>
+      <c r="AU11">
+        <v>15.83333333333333</v>
+      </c>
+      <c r="AV11">
+        <v>19.4</v>
+      </c>
+      <c r="AW11">
+        <v>94</v>
+      </c>
+      <c r="AX11">
+        <v>18.73246766019657</v>
+      </c>
+      <c r="AY11">
+        <v>10.16469840167657</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update results to use consistent baseline for approah 3b
</commit_message>
<xml_diff>
--- a/data/outputs/full_results/summary_results_all.xlsx
+++ b/data/outputs/full_results/summary_results_all.xlsx
@@ -1273,25 +1273,25 @@
         <v>120.1679757883243</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
         <v>4</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>5</v>
       </c>
-      <c r="M6">
-        <v>6</v>
-      </c>
       <c r="N6">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="O6">
-        <v>7.981012658227848</v>
+        <v>7.319620253164557</v>
       </c>
       <c r="P6">
-        <v>8.594181508245255</v>
+        <v>8.506340931670369</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -1303,16 +1303,16 @@
         <v>1</v>
       </c>
       <c r="T6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U6">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V6">
-        <v>2.512658227848101</v>
+        <v>2.810126582278481</v>
       </c>
       <c r="W6">
-        <v>4.48098251948876</v>
+        <v>4.972498204788462</v>
       </c>
       <c r="X6">
         <v>0</v>
@@ -1327,13 +1327,13 @@
         <v>0</v>
       </c>
       <c r="AB6">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="AC6">
-        <v>1.069620253164557</v>
+        <v>1.338607594936709</v>
       </c>
       <c r="AD6">
-        <v>3.073939798870591</v>
+        <v>4.130709223604813</v>
       </c>
       <c r="AE6">
         <v>0</v>
@@ -1351,52 +1351,52 @@
         <v>2</v>
       </c>
       <c r="AJ6">
-        <v>0.120253164556962</v>
+        <v>0.129746835443038</v>
       </c>
       <c r="AK6">
-        <v>0.3447123472852491</v>
+        <v>0.3637563275916581</v>
       </c>
       <c r="AL6">
-        <v>0.6666666666666666</v>
+        <v>0</v>
       </c>
       <c r="AM6">
-        <v>1.5</v>
+        <v>1.473684210526316</v>
       </c>
       <c r="AN6">
         <v>2</v>
       </c>
       <c r="AO6">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AP6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AQ6">
-        <v>2.290964753656293</v>
+        <v>1.949513816186035</v>
       </c>
       <c r="AR6">
-        <v>0.9224471218358076</v>
+        <v>0.712827936278364</v>
       </c>
       <c r="AS6">
-        <v>9.333333333333334</v>
+        <v>11.56756756756757</v>
       </c>
       <c r="AT6">
-        <v>13.57142857142857</v>
+        <v>15.8125</v>
       </c>
       <c r="AU6">
-        <v>15.83333333333333</v>
+        <v>17.41666666666666</v>
       </c>
       <c r="AV6">
-        <v>19</v>
+        <v>19.4</v>
       </c>
       <c r="AW6">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="AX6">
-        <v>16.53393065646352</v>
+        <v>18.53251213318498</v>
       </c>
       <c r="AY6">
-        <v>4.521254120415229</v>
+        <v>5.580829287170561</v>
       </c>
     </row>
     <row r="7">
@@ -2064,19 +2064,19 @@
         <v>4</v>
       </c>
       <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="M11">
         <v>6</v>
       </c>
-      <c r="M11">
-        <v>7</v>
-      </c>
       <c r="N11">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O11">
-        <v>7.377952755905512</v>
+        <v>6.55511811023622</v>
       </c>
       <c r="P11">
-        <v>5.779107982453519</v>
+        <v>5.867687475497098</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -2088,16 +2088,16 @@
         <v>2</v>
       </c>
       <c r="T11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U11">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="V11">
-        <v>3.216535433070866</v>
+        <v>3.204724409448819</v>
       </c>
       <c r="W11">
-        <v>3.275909523513953</v>
+        <v>3.530417979435353</v>
       </c>
       <c r="X11">
         <v>0</v>
@@ -2112,76 +2112,76 @@
         <v>0</v>
       </c>
       <c r="AB11">
+        <v>26</v>
+      </c>
+      <c r="AC11">
+        <v>2.122047244094488</v>
+      </c>
+      <c r="AD11">
+        <v>4.446083027817777</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <v>2</v>
+      </c>
+      <c r="AJ11">
+        <v>0.2322834645669291</v>
+      </c>
+      <c r="AK11">
+        <v>0.4758818549636049</v>
+      </c>
+      <c r="AL11">
+        <v>0</v>
+      </c>
+      <c r="AM11">
+        <v>1.157894736842105</v>
+      </c>
+      <c r="AN11">
+        <v>2</v>
+      </c>
+      <c r="AO11">
+        <v>2.5</v>
+      </c>
+      <c r="AP11">
+        <v>4</v>
+      </c>
+      <c r="AQ11">
+        <v>1.812612239259566</v>
+      </c>
+      <c r="AR11">
+        <v>0.858066687701709</v>
+      </c>
+      <c r="AS11">
+        <v>10.55555555555556</v>
+      </c>
+      <c r="AT11">
+        <v>15.83333333333333</v>
+      </c>
+      <c r="AU11">
         <v>19</v>
       </c>
-      <c r="AC11">
-        <v>1.803149606299213</v>
-      </c>
-      <c r="AD11">
-        <v>3.905078015807789</v>
-      </c>
-      <c r="AE11">
-        <v>0</v>
-      </c>
-      <c r="AF11">
-        <v>0</v>
-      </c>
-      <c r="AG11">
-        <v>0</v>
-      </c>
-      <c r="AH11">
-        <v>0</v>
-      </c>
-      <c r="AI11">
-        <v>2</v>
-      </c>
-      <c r="AJ11">
-        <v>0.2007874015748032</v>
-      </c>
-      <c r="AK11">
-        <v>0.4299087251214076</v>
-      </c>
-      <c r="AL11">
-        <v>0</v>
-      </c>
-      <c r="AM11">
-        <v>1.333333333333333</v>
-      </c>
-      <c r="AN11">
-        <v>2</v>
-      </c>
-      <c r="AO11">
-        <v>3</v>
-      </c>
-      <c r="AP11">
-        <v>4.5</v>
-      </c>
-      <c r="AQ11">
-        <v>2.192074674876167</v>
-      </c>
-      <c r="AR11">
-        <v>1.038702278113778</v>
-      </c>
-      <c r="AS11">
-        <v>9.5</v>
-      </c>
-      <c r="AT11">
-        <v>13.57142857142857</v>
-      </c>
-      <c r="AU11">
-        <v>15.83333333333333</v>
-      </c>
       <c r="AV11">
-        <v>19.4</v>
+        <v>23.75</v>
       </c>
       <c r="AW11">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AX11">
-        <v>18.73246766019657</v>
+        <v>22.00835514543718</v>
       </c>
       <c r="AY11">
-        <v>10.16469840167657</v>
+        <v>13.28140617026885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update perf_series, limits_table, summary_results and full_results to reflect latest versions
</commit_message>
<xml_diff>
--- a/data/outputs/full_results/summary_results_all.xlsx
+++ b/data/outputs/full_results/summary_results_all.xlsx
@@ -669,49 +669,49 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="S2">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="T2">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="U2">
-        <v>71</v>
+        <v>127</v>
       </c>
       <c r="V2">
-        <v>18.74050632911392</v>
+        <v>25.93354430379747</v>
       </c>
       <c r="W2">
-        <v>11.48950128346818</v>
+        <v>18.59421350768726</v>
       </c>
       <c r="X2">
         <v>0</v>
       </c>
       <c r="Y2">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="Z2">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="AA2">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="AB2">
-        <v>132</v>
+        <v>231</v>
       </c>
       <c r="AC2">
-        <v>32.06962025316456</v>
+        <v>47.5759493670886</v>
       </c>
       <c r="AD2">
-        <v>17.510130252018</v>
+        <v>39.54339297110542</v>
       </c>
       <c r="AE2">
         <v>0</v>
       </c>
       <c r="AF2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG2">
         <v>2</v>
@@ -720,13 +720,13 @@
         <v>3</v>
       </c>
       <c r="AI2">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="AJ2">
-        <v>1.857594936708861</v>
+        <v>3.139240506329114</v>
       </c>
       <c r="AK2">
-        <v>1.127705596152351</v>
+        <v>2.773956785304159</v>
       </c>
       <c r="AL2">
         <v>0</v>
@@ -1140,64 +1140,64 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="S5">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="T5">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="U5">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="V5">
-        <v>15.37658227848101</v>
+        <v>21.94303797468354</v>
       </c>
       <c r="W5">
-        <v>10.69819547294476</v>
+        <v>15.23706578047602</v>
       </c>
       <c r="X5">
         <v>0</v>
       </c>
       <c r="Y5">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="Z5">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="AA5">
-        <v>39</v>
+        <v>53.25</v>
       </c>
       <c r="AB5">
-        <v>67</v>
+        <v>174</v>
       </c>
       <c r="AC5">
-        <v>30.38291139240506</v>
+        <v>45.81645569620253</v>
       </c>
       <c r="AD5">
-        <v>14.28670907727845</v>
+        <v>32.42374959615592</v>
       </c>
       <c r="AE5">
         <v>0</v>
       </c>
       <c r="AF5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG5">
         <v>2</v>
       </c>
       <c r="AH5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI5">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="AJ5">
-        <v>1.629746835443038</v>
+        <v>3.09493670886076</v>
       </c>
       <c r="AK5">
-        <v>0.8867282108014968</v>
+        <v>2.567904400840213</v>
       </c>
       <c r="AL5">
         <v>0</v>
@@ -1297,64 +1297,64 @@
         <v>0</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S6">
+        <v>7</v>
+      </c>
+      <c r="T6">
+        <v>12</v>
+      </c>
+      <c r="U6">
+        <v>65</v>
+      </c>
+      <c r="V6">
+        <v>9.79746835443038</v>
+      </c>
+      <c r="W6">
+        <v>10.04419408615073</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>8</v>
+      </c>
+      <c r="AA6">
+        <v>11</v>
+      </c>
+      <c r="AB6">
+        <v>43</v>
+      </c>
+      <c r="AC6">
+        <v>8.018987341772151</v>
+      </c>
+      <c r="AD6">
+        <v>9.248232104921779</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
         <v>1</v>
       </c>
-      <c r="T6">
-        <v>3</v>
-      </c>
-      <c r="U6">
-        <v>37</v>
-      </c>
-      <c r="V6">
-        <v>2.357594936708861</v>
-      </c>
-      <c r="W6">
-        <v>4.071812424403884</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6">
-        <v>0</v>
-      </c>
-      <c r="AB6">
-        <v>34</v>
-      </c>
-      <c r="AC6">
-        <v>1.30379746835443</v>
-      </c>
-      <c r="AD6">
-        <v>4.112248619436459</v>
-      </c>
-      <c r="AE6">
-        <v>0</v>
-      </c>
-      <c r="AF6">
-        <v>0</v>
-      </c>
-      <c r="AG6">
-        <v>0</v>
-      </c>
       <c r="AH6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI6">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AJ6">
-        <v>0.129746835443038</v>
+        <v>0.8069620253164557</v>
       </c>
       <c r="AK6">
-        <v>0.3723813532014942</v>
+        <v>0.9036516458049771</v>
       </c>
       <c r="AL6">
         <v>0</v>
@@ -1454,64 +1454,64 @@
         <v>0</v>
       </c>
       <c r="R7">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="S7">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="T7">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="U7">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="V7">
-        <v>18.60995850622407</v>
+        <v>25.67219917012448</v>
       </c>
       <c r="W7">
-        <v>12.53184877614916</v>
+        <v>13.9754403231824</v>
       </c>
       <c r="X7">
         <v>0</v>
       </c>
       <c r="Y7">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="Z7">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="AA7">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="AB7">
-        <v>74</v>
+        <v>174</v>
       </c>
       <c r="AC7">
-        <v>28.30705394190871</v>
+        <v>39.25311203319502</v>
       </c>
       <c r="AD7">
-        <v>16.32779812777108</v>
+        <v>21.75350164973208</v>
       </c>
       <c r="AE7">
         <v>0</v>
       </c>
       <c r="AF7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI7">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="AJ7">
-        <v>1.809128630705394</v>
+        <v>2.809128630705394</v>
       </c>
       <c r="AK7">
-        <v>1.031220791530699</v>
+        <v>1.608855593546295</v>
       </c>
       <c r="AL7">
         <v>0</v>
@@ -1925,64 +1925,64 @@
         <v>0</v>
       </c>
       <c r="R10">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="S10">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="T10">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="U10">
         <v>57</v>
       </c>
       <c r="V10">
-        <v>17.21161825726141</v>
+        <v>23.28630705394191</v>
       </c>
       <c r="W10">
-        <v>11.60714712811315</v>
+        <v>10.94745876396246</v>
       </c>
       <c r="X10">
         <v>0</v>
       </c>
       <c r="Y10">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="Z10">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="AA10">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="AB10">
-        <v>64</v>
+        <v>141</v>
       </c>
       <c r="AC10">
-        <v>26.58921161825726</v>
+        <v>36.87966804979253</v>
       </c>
       <c r="AD10">
-        <v>15.0053229375178</v>
+        <v>20.00453181713292</v>
       </c>
       <c r="AE10">
         <v>0</v>
       </c>
       <c r="AF10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG10">
         <v>2</v>
       </c>
       <c r="AH10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI10">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="AJ10">
-        <v>1.651452282157676</v>
+        <v>2.701244813278008</v>
       </c>
       <c r="AK10">
-        <v>0.9145171578972808</v>
+        <v>1.597510597977387</v>
       </c>
       <c r="AL10">
         <v>0</v>
@@ -2082,64 +2082,64 @@
         <v>0</v>
       </c>
       <c r="R11">
+        <v>6</v>
+      </c>
+      <c r="S11">
+        <v>12</v>
+      </c>
+      <c r="T11">
+        <v>19</v>
+      </c>
+      <c r="U11">
+        <v>112</v>
+      </c>
+      <c r="V11">
+        <v>15.01244813278008</v>
+      </c>
+      <c r="W11">
+        <v>14.51019220174818</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>9</v>
+      </c>
+      <c r="AA11">
+        <v>17</v>
+      </c>
+      <c r="AB11">
+        <v>35</v>
+      </c>
+      <c r="AC11">
+        <v>9.95850622406639</v>
+      </c>
+      <c r="AD11">
+        <v>8.95441815117</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
         <v>1</v>
       </c>
-      <c r="S11">
+      <c r="AH11">
         <v>2</v>
       </c>
-      <c r="T11">
+      <c r="AI11">
         <v>4</v>
       </c>
-      <c r="U11">
-        <v>57</v>
-      </c>
-      <c r="V11">
-        <v>3.020746887966805</v>
-      </c>
-      <c r="W11">
-        <v>4.500414918630728</v>
-      </c>
-      <c r="X11">
-        <v>0</v>
-      </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
-      <c r="Z11">
-        <v>0</v>
-      </c>
-      <c r="AA11">
-        <v>0</v>
-      </c>
-      <c r="AB11">
-        <v>21</v>
-      </c>
-      <c r="AC11">
-        <v>2.058091286307054</v>
-      </c>
-      <c r="AD11">
-        <v>4.183891092627223</v>
-      </c>
-      <c r="AE11">
-        <v>0</v>
-      </c>
-      <c r="AF11">
-        <v>0</v>
-      </c>
-      <c r="AG11">
-        <v>0</v>
-      </c>
-      <c r="AH11">
-        <v>0</v>
-      </c>
-      <c r="AI11">
-        <v>2</v>
-      </c>
       <c r="AJ11">
-        <v>0.2240663900414938</v>
+        <v>1.04149377593361</v>
       </c>
       <c r="AK11">
-        <v>0.4467494401123116</v>
+        <v>0.9210163368091974</v>
       </c>
       <c r="AL11">
         <v>0</v>

</xml_diff>

<commit_message>
Correct data update following autospc v0.0.0.9030
</commit_message>
<xml_diff>
--- a/data/outputs/full_results/summary_results_all.xlsx
+++ b/data/outputs/full_results/summary_results_all.xlsx
@@ -660,52 +660,52 @@
         <v>14</v>
       </c>
       <c r="O2">
-        <v>2.39873417721519</v>
+        <v>2.300632911392405</v>
       </c>
       <c r="P2">
-        <v>3.163160712672262</v>
+        <v>3.145387085179154</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="S2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U2">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="V2">
-        <v>25.93354430379747</v>
+        <v>26.66455696202532</v>
       </c>
       <c r="W2">
-        <v>18.59421350768726</v>
+        <v>18.32999476423991</v>
       </c>
       <c r="X2">
         <v>0</v>
       </c>
       <c r="Y2">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="Z2">
-        <v>38</v>
+        <v>39.5</v>
       </c>
       <c r="AA2">
-        <v>53</v>
+        <v>53.25</v>
       </c>
       <c r="AB2">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="AC2">
-        <v>47.5759493670886</v>
+        <v>49.1740506329114</v>
       </c>
       <c r="AD2">
-        <v>39.54339297110542</v>
+        <v>39.89666920159571</v>
       </c>
       <c r="AE2">
         <v>0</v>
@@ -720,19 +720,19 @@
         <v>3</v>
       </c>
       <c r="AI2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AJ2">
-        <v>3.139240506329114</v>
+        <v>3.164556962025316</v>
       </c>
       <c r="AK2">
-        <v>2.773956785304159</v>
+        <v>2.82249638349463</v>
       </c>
       <c r="AL2">
         <v>0</v>
       </c>
       <c r="AM2">
-        <v>0.3684210526315789</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="AN2">
         <v>0.5</v>
@@ -744,31 +744,31 @@
         <v>1</v>
       </c>
       <c r="AQ2">
-        <v>0.5718053044002411</v>
+        <v>0.5307215824371054</v>
       </c>
       <c r="AR2">
-        <v>0.3491428476565057</v>
+        <v>0.3479943612339447</v>
       </c>
       <c r="AS2">
-        <v>24</v>
+        <v>24.25</v>
       </c>
       <c r="AT2">
         <v>31.66666666666667</v>
       </c>
       <c r="AU2">
-        <v>46</v>
+        <v>47.5</v>
       </c>
       <c r="AV2">
-        <v>48</v>
+        <v>48.5</v>
       </c>
       <c r="AW2">
         <v>97</v>
       </c>
       <c r="AX2">
-        <v>44.97944839970157</v>
+        <v>47.07499209651108</v>
       </c>
       <c r="AY2">
-        <v>16.92484101997347</v>
+        <v>18.10781587709074</v>
       </c>
     </row>
     <row r="3">
@@ -838,16 +838,16 @@
         <v>234</v>
       </c>
       <c r="V3">
-        <v>43.53164556962025</v>
+        <v>43.45569620253165</v>
       </c>
       <c r="W3">
-        <v>38.9090385526683</v>
+        <v>38.9706596897797</v>
       </c>
       <c r="X3">
         <v>0</v>
       </c>
       <c r="Y3">
-        <v>48</v>
+        <v>47.75</v>
       </c>
       <c r="Z3">
         <v>66.5</v>
@@ -859,10 +859,10 @@
         <v>388</v>
       </c>
       <c r="AC3">
-        <v>92.26582278481013</v>
+        <v>92.11075949367088</v>
       </c>
       <c r="AD3">
-        <v>84.12544810392367</v>
+        <v>84.25051690139057</v>
       </c>
       <c r="AE3">
         <v>0</v>
@@ -880,10 +880,10 @@
         <v>19</v>
       </c>
       <c r="AJ3">
-        <v>4.208860759493671</v>
+        <v>4.193037974683544</v>
       </c>
       <c r="AK3">
-        <v>4.034067304281272</v>
+        <v>4.040754559247215</v>
       </c>
       <c r="AL3">
         <v>0</v>
@@ -1119,7 +1119,7 @@
         <v>0</v>
       </c>
       <c r="K5">
-        <v>1.75</v>
+        <v>1</v>
       </c>
       <c r="L5">
         <v>2</v>
@@ -1128,13 +1128,13 @@
         <v>2</v>
       </c>
       <c r="N5">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="O5">
-        <v>3.541139240506329</v>
+        <v>3.522151898734177</v>
       </c>
       <c r="P5">
-        <v>4.576844823596349</v>
+        <v>4.576282866961004</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -1146,64 +1146,64 @@
         <v>19</v>
       </c>
       <c r="T5">
-        <v>29</v>
+        <v>29.25</v>
       </c>
       <c r="U5">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="V5">
-        <v>21.94303797468354</v>
+        <v>21.92721518987342</v>
       </c>
       <c r="W5">
-        <v>15.23706578047602</v>
+        <v>15.29262982038693</v>
       </c>
       <c r="X5">
         <v>0</v>
       </c>
       <c r="Y5">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Z5">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AA5">
-        <v>53.25</v>
+        <v>54</v>
       </c>
       <c r="AB5">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="AC5">
-        <v>45.81645569620253</v>
+        <v>46.2626582278481</v>
       </c>
       <c r="AD5">
-        <v>32.42374959615592</v>
+        <v>32.5537016336737</v>
       </c>
       <c r="AE5">
         <v>0</v>
       </c>
       <c r="AF5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG5">
         <v>2</v>
       </c>
       <c r="AH5">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="AI5">
         <v>15</v>
       </c>
       <c r="AJ5">
-        <v>3.09493670886076</v>
+        <v>3.091772151898734</v>
       </c>
       <c r="AK5">
-        <v>2.567904400840213</v>
+        <v>2.610320546876234</v>
       </c>
       <c r="AL5">
         <v>0</v>
       </c>
       <c r="AM5">
-        <v>0.6842105263157895</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AN5">
         <v>1</v>
@@ -1215,13 +1215,13 @@
         <v>1</v>
       </c>
       <c r="AQ5">
-        <v>0.8488309381047555</v>
+        <v>0.8365335807874116</v>
       </c>
       <c r="AR5">
-        <v>0.2356354939144961</v>
+        <v>0.251086959137955</v>
       </c>
       <c r="AS5">
-        <v>22.52631578947368</v>
+        <v>23.77777777777778</v>
       </c>
       <c r="AT5">
         <v>31.33333333333333</v>
@@ -1236,10 +1236,10 @@
         <v>61</v>
       </c>
       <c r="AX5">
-        <v>32.70385789217205</v>
+        <v>33.03482243432914</v>
       </c>
       <c r="AY5">
-        <v>6.259984126916317</v>
+        <v>6.477471883527956</v>
       </c>
     </row>
     <row r="6">
@@ -1288,10 +1288,10 @@
         <v>36</v>
       </c>
       <c r="O6">
-        <v>7.262658227848101</v>
+        <v>7.186708860759493</v>
       </c>
       <c r="P6">
-        <v>8.559261087950867</v>
+        <v>8.515901871767431</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -1303,16 +1303,16 @@
         <v>7</v>
       </c>
       <c r="T6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="U6">
         <v>65</v>
       </c>
       <c r="V6">
-        <v>9.79746835443038</v>
+        <v>9.882911392405063</v>
       </c>
       <c r="W6">
-        <v>10.04419408615073</v>
+        <v>9.952054541255478</v>
       </c>
       <c r="X6">
         <v>0</v>
@@ -1324,16 +1324,16 @@
         <v>8</v>
       </c>
       <c r="AA6">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="AB6">
         <v>43</v>
       </c>
       <c r="AC6">
-        <v>8.018987341772151</v>
+        <v>9.113924050632912</v>
       </c>
       <c r="AD6">
-        <v>9.248232104921779</v>
+        <v>9.847713252272086</v>
       </c>
       <c r="AE6">
         <v>0</v>
@@ -1345,22 +1345,22 @@
         <v>1</v>
       </c>
       <c r="AH6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI6">
         <v>5</v>
       </c>
       <c r="AJ6">
-        <v>0.8069620253164557</v>
+        <v>0.9240506329113924</v>
       </c>
       <c r="AK6">
-        <v>0.9036516458049771</v>
+        <v>0.9729307960672774</v>
       </c>
       <c r="AL6">
         <v>0</v>
       </c>
       <c r="AM6">
-        <v>1.493421052631579</v>
+        <v>1.473684210526316</v>
       </c>
       <c r="AN6">
         <v>2</v>
@@ -1369,13 +1369,13 @@
         <v>2.5</v>
       </c>
       <c r="AP6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AQ6">
-        <v>1.91289933694997</v>
+        <v>1.881864471304844</v>
       </c>
       <c r="AR6">
-        <v>0.6949275979472178</v>
+        <v>0.6722739449024928</v>
       </c>
       <c r="AS6">
         <v>11.56756756756757</v>
@@ -1384,19 +1384,19 @@
         <v>15.83333333333333</v>
       </c>
       <c r="AU6">
-        <v>17.83333333333333</v>
+        <v>18.60869565217391</v>
       </c>
       <c r="AV6">
-        <v>19.45454545454545</v>
+        <v>20.08333333333333</v>
       </c>
       <c r="AW6">
         <v>59</v>
       </c>
       <c r="AX6">
-        <v>18.85424829140588</v>
+        <v>19.04728065130852</v>
       </c>
       <c r="AY6">
-        <v>5.919295038457036</v>
+        <v>5.882771635131574</v>
       </c>
     </row>
     <row r="7">
@@ -1445,16 +1445,16 @@
         <v>12</v>
       </c>
       <c r="O7">
-        <v>2.763485477178423</v>
+        <v>2.738589211618257</v>
       </c>
       <c r="P7">
-        <v>3.231046445683381</v>
+        <v>3.207108718880054</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="S7">
         <v>25</v>
@@ -1466,10 +1466,10 @@
         <v>108</v>
       </c>
       <c r="V7">
-        <v>25.67219917012448</v>
+        <v>25.85477178423237</v>
       </c>
       <c r="W7">
-        <v>13.9754403231824</v>
+        <v>13.93645056025866</v>
       </c>
       <c r="X7">
         <v>0</v>
@@ -1478,7 +1478,7 @@
         <v>26</v>
       </c>
       <c r="Z7">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AA7">
         <v>49</v>
@@ -1487,10 +1487,10 @@
         <v>174</v>
       </c>
       <c r="AC7">
-        <v>39.25311203319502</v>
+        <v>39.8298755186722</v>
       </c>
       <c r="AD7">
-        <v>21.75350164973208</v>
+        <v>21.95108434074362</v>
       </c>
       <c r="AE7">
         <v>0</v>
@@ -1508,31 +1508,31 @@
         <v>11</v>
       </c>
       <c r="AJ7">
-        <v>2.809128630705394</v>
+        <v>2.842323651452282</v>
       </c>
       <c r="AK7">
-        <v>1.608855593546295</v>
+        <v>1.655808335772374</v>
       </c>
       <c r="AL7">
         <v>0</v>
       </c>
       <c r="AM7">
-        <v>0.4736842105263158</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="AN7">
         <v>0.5</v>
       </c>
       <c r="AO7">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="AP7">
         <v>1</v>
       </c>
       <c r="AQ7">
-        <v>0.5842198858141203</v>
+        <v>0.5773406545409167</v>
       </c>
       <c r="AR7">
-        <v>0.2999429303817278</v>
+        <v>0.2964972793141106</v>
       </c>
       <c r="AS7">
         <v>24.25</v>
@@ -1541,7 +1541,7 @@
         <v>32.33333333333334</v>
       </c>
       <c r="AU7">
-        <v>46.5</v>
+        <v>47.5</v>
       </c>
       <c r="AV7">
         <v>47.5</v>
@@ -1550,10 +1550,10 @@
         <v>97</v>
       </c>
       <c r="AX7">
-        <v>44.20441695234226</v>
+        <v>44.44608321600023</v>
       </c>
       <c r="AY7">
-        <v>15.47073349176565</v>
+        <v>15.39743138309131</v>
       </c>
     </row>
     <row r="8">
@@ -1611,10 +1611,10 @@
         <v>0</v>
       </c>
       <c r="R8">
-        <v>6.25</v>
+        <v>0</v>
       </c>
       <c r="S8">
-        <v>39</v>
+        <v>38.5</v>
       </c>
       <c r="T8">
         <v>57</v>
@@ -1623,16 +1623,16 @@
         <v>330</v>
       </c>
       <c r="V8">
-        <v>49.60429447852761</v>
+        <v>49.15644171779141</v>
       </c>
       <c r="W8">
-        <v>63.39012187029993</v>
+        <v>63.67318047830457</v>
       </c>
       <c r="X8">
         <v>0</v>
       </c>
       <c r="Y8">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="Z8">
         <v>67</v>
@@ -1644,16 +1644,16 @@
         <v>398</v>
       </c>
       <c r="AC8">
-        <v>84.65644171779141</v>
+        <v>83.8159509202454</v>
       </c>
       <c r="AD8">
-        <v>100.432534132236</v>
+        <v>101.0177890968519</v>
       </c>
       <c r="AE8">
         <v>0</v>
       </c>
       <c r="AF8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG8">
         <v>3</v>
@@ -1665,10 +1665,10 @@
         <v>16</v>
       </c>
       <c r="AJ8">
-        <v>3.254601226993865</v>
+        <v>3.187116564417178</v>
       </c>
       <c r="AK8">
-        <v>2.939318653733056</v>
+        <v>2.988998231757231</v>
       </c>
       <c r="AL8">
         <v>0</v>
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <v>2</v>
@@ -1916,10 +1916,10 @@
         <v>16</v>
       </c>
       <c r="O10">
-        <v>3.423236514522821</v>
+        <v>3.402489626556016</v>
       </c>
       <c r="P10">
-        <v>3.872353868298687</v>
+        <v>3.883704474158696</v>
       </c>
       <c r="Q10">
         <v>0</v>
@@ -1937,10 +1937,10 @@
         <v>57</v>
       </c>
       <c r="V10">
-        <v>23.28630705394191</v>
+        <v>23.44398340248962</v>
       </c>
       <c r="W10">
-        <v>10.94745876396246</v>
+        <v>10.74311674514074</v>
       </c>
       <c r="X10">
         <v>0</v>
@@ -1952,16 +1952,16 @@
         <v>35</v>
       </c>
       <c r="AA10">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AB10">
         <v>141</v>
       </c>
       <c r="AC10">
-        <v>36.87966804979253</v>
+        <v>37.43568464730291</v>
       </c>
       <c r="AD10">
-        <v>20.00453181713292</v>
+        <v>20.12867493486523</v>
       </c>
       <c r="AE10">
         <v>0</v>
@@ -1979,10 +1979,10 @@
         <v>10</v>
       </c>
       <c r="AJ10">
-        <v>2.701244813278008</v>
+        <v>2.692946058091287</v>
       </c>
       <c r="AK10">
-        <v>1.597510597977387</v>
+        <v>1.601142831827155</v>
       </c>
       <c r="AL10">
         <v>0</v>
@@ -1991,7 +1991,7 @@
         <v>0.5</v>
       </c>
       <c r="AN10">
-        <v>0.7894736842105263</v>
+        <v>0.7368421052631579</v>
       </c>
       <c r="AO10">
         <v>1</v>
@@ -2000,10 +2000,10 @@
         <v>1</v>
       </c>
       <c r="AQ10">
-        <v>0.7550463295167379</v>
+        <v>0.7439813226011086</v>
       </c>
       <c r="AR10">
-        <v>0.2743716149123772</v>
+        <v>0.2806086267855832</v>
       </c>
       <c r="AS10">
         <v>24.25</v>
@@ -2015,16 +2015,16 @@
         <v>31.66666666666667</v>
       </c>
       <c r="AV10">
-        <v>38</v>
+        <v>42.8</v>
       </c>
       <c r="AW10">
         <v>95</v>
       </c>
       <c r="AX10">
-        <v>36.73393507070588</v>
+        <v>37.10115498771832</v>
       </c>
       <c r="AY10">
-        <v>11.05411732317182</v>
+        <v>11.126796191337</v>
       </c>
     </row>
     <row r="11">
@@ -2070,13 +2070,13 @@
         <v>6</v>
       </c>
       <c r="N11">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O11">
-        <v>7</v>
+        <v>6.950207468879668</v>
       </c>
       <c r="P11">
-        <v>5.911852501542981</v>
+        <v>5.845725820926259</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -2094,10 +2094,10 @@
         <v>112</v>
       </c>
       <c r="V11">
-        <v>15.01244813278008</v>
+        <v>15.09128630705394</v>
       </c>
       <c r="W11">
-        <v>14.51019220174818</v>
+        <v>14.51952589062467</v>
       </c>
       <c r="X11">
         <v>0</v>
@@ -2112,13 +2112,13 @@
         <v>17</v>
       </c>
       <c r="AB11">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="AC11">
-        <v>9.95850622406639</v>
+        <v>10.46058091286307</v>
       </c>
       <c r="AD11">
-        <v>8.95441815117</v>
+        <v>9.324670574760313</v>
       </c>
       <c r="AE11">
         <v>0</v>
@@ -2133,13 +2133,13 @@
         <v>2</v>
       </c>
       <c r="AI11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AJ11">
-        <v>1.04149377593361</v>
+        <v>1.095435684647303</v>
       </c>
       <c r="AK11">
-        <v>0.9210163368091974</v>
+        <v>0.9721217757503259</v>
       </c>
       <c r="AL11">
         <v>0</v>
@@ -2157,19 +2157,19 @@
         <v>4</v>
       </c>
       <c r="AQ11">
-        <v>1.932096839609397</v>
+        <v>1.917173639492923</v>
       </c>
       <c r="AR11">
-        <v>0.8394779094682686</v>
+        <v>0.8280222081088773</v>
       </c>
       <c r="AS11">
         <v>10.55555555555556</v>
       </c>
       <c r="AT11">
-        <v>14.26666666666667</v>
+        <v>14.66666666666667</v>
       </c>
       <c r="AU11">
-        <v>17.83333333333333</v>
+        <v>18.6</v>
       </c>
       <c r="AV11">
         <v>20.38095238095238</v>
@@ -2178,10 +2178,10 @@
         <v>94</v>
       </c>
       <c r="AX11">
-        <v>19.87290317920228</v>
+        <v>19.95054735876594</v>
       </c>
       <c r="AY11">
-        <v>9.866064184366177</v>
+        <v>9.828944512850548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>